<commit_message>
25-11-2017:Updated With Date Logic
</commit_message>
<xml_diff>
--- a/Society/CustomerApp/Docs/TestCase(AutoRecovered).xlsx
+++ b/Society/CustomerApp/Docs/TestCase(AutoRecovered).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="811" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="811" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="4" r:id="rId1"/>
@@ -21,8 +21,10 @@
     <sheet name="Loan_Report" sheetId="7" r:id="rId7"/>
     <sheet name="meeting_nobook" sheetId="5" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">loan_nobook!$A$1:$F$12</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -880,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="D1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -1118,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -1303,7 +1305,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -1554,10 +1556,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -1590,7 +1593,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A2">
         <v>3.3</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A3">
         <v>3.5</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>43069</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A4">
         <v>3.5</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>43069</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A5">
         <v>3.7</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A6">
         <v>3.7</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A8">
         <v>3.9</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A10">
         <v>3.9</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.7">
       <c r="A11">
         <v>3.9</v>
       </c>
@@ -1778,6 +1781,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F12">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Q"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1787,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -2106,7 +2116,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>

</xml_diff>